<commit_message>
build(files): a lot changed and updated.
</commit_message>
<xml_diff>
--- a/results/min_var_portfolio/min_var_2011.xlsx
+++ b/results/min_var_portfolio/min_var_2011.xlsx
@@ -531,7 +531,7 @@
         <v>0.01764933193576036</v>
       </c>
       <c r="N2" t="n">
-        <v>0.001</v>
+        <v>0.03391593108946795</v>
       </c>
     </row>
     <row r="3">
@@ -577,7 +577,7 @@
         <v>0.1024159248621946</v>
       </c>
       <c r="N3" t="n">
-        <v>0.001000000000000009</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="4">
@@ -623,7 +623,7 @@
         <v>0.04053633029405575</v>
       </c>
       <c r="N4" t="n">
-        <v>0.001000000000000021</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="5">
@@ -669,7 +669,7 @@
         <v>0.02518322987560368</v>
       </c>
       <c r="N5" t="n">
-        <v>0.001</v>
+        <v>0.01583706974633639</v>
       </c>
     </row>
     <row r="6">
@@ -715,7 +715,7 @@
         <v>0.0264056187940291</v>
       </c>
       <c r="N6" t="n">
-        <v>0.3374133971524808</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="7">
@@ -761,7 +761,7 @@
         <v>-0.03715286740634847</v>
       </c>
       <c r="N7" t="n">
-        <v>0.00100000000000001</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="8">
@@ -807,7 +807,7 @@
         <v>0.03389144603653566</v>
       </c>
       <c r="N8" t="n">
-        <v>0.001</v>
+        <v>0.06185955134729807</v>
       </c>
     </row>
     <row r="9">
@@ -853,7 +853,7 @@
         <v>0.009682415320185407</v>
       </c>
       <c r="N9" t="n">
-        <v>0.001</v>
+        <v>0.005090972792413145</v>
       </c>
     </row>
     <row r="10">
@@ -899,7 +899,7 @@
         <v>0.04101796640782445</v>
       </c>
       <c r="N10" t="n">
-        <v>0.001000000000000008</v>
+        <v>0.001000000000000019</v>
       </c>
     </row>
     <row r="11">
@@ -945,7 +945,7 @@
         <v>-0.06140485719980725</v>
       </c>
       <c r="N11" t="n">
-        <v>0.2969605761064857</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="12">
@@ -991,7 +991,7 @@
         <v>0.01816450975952328</v>
       </c>
       <c r="N12" t="n">
-        <v>0.001</v>
+        <v>0.02867792884142787</v>
       </c>
     </row>
     <row r="13">
@@ -1037,7 +1037,7 @@
         <v>0.1144668619218644</v>
       </c>
       <c r="N13" t="n">
-        <v>0.001</v>
+        <v>0.095365390944626</v>
       </c>
     </row>
     <row r="14">
@@ -1083,7 +1083,7 @@
         <v>-0.07128952566974377</v>
       </c>
       <c r="N14" t="n">
-        <v>0.001</v>
+        <v>0.001253155238430658</v>
       </c>
     </row>
     <row r="15">
@@ -1175,7 +1175,7 @@
         <v>0.02234718276350268</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1645456221732258</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="17">
@@ -1221,7 +1221,7 @@
         <v>-0.001597699652852412</v>
       </c>
       <c r="N17" t="n">
-        <v>0.07720024067766219</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="18">
@@ -1313,7 +1313,7 @@
         <v>0.09710074087900096</v>
       </c>
       <c r="N19" t="n">
-        <v>0.1088801638901456</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="20">
@@ -1359,7 +1359,7 @@
         <v>0.02367374678372322</v>
       </c>
       <c r="N20" t="n">
-        <v>0.001000000000000007</v>
+        <v>0.001000000000000008</v>
       </c>
     </row>
     <row r="21">
@@ -1405,7 +1405,7 @@
         <v>-0.03537346297258082</v>
       </c>
       <c r="N21" t="n">
-        <v>0.001000000000000009</v>
+        <v>0.001000000000000014</v>
       </c>
     </row>
     <row r="22">
@@ -1415,40 +1415,40 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.008611052412310645</v>
+        <v>-0.000915621970130807</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01805754227438011</v>
+        <v>0.0319937614770624</v>
       </c>
       <c r="D22" t="n">
-        <v>0.001969951216531318</v>
+        <v>0.009365989214743591</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01479149785066426</v>
+        <v>0.0177354452815994</v>
       </c>
       <c r="F22" t="n">
-        <v>0.03227885793565562</v>
+        <v>0.04298969661505471</v>
       </c>
       <c r="G22" t="n">
-        <v>0.04907800704042601</v>
+        <v>0.06497452557344659</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.009398871864275089</v>
+        <v>0.01501434834603236</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.003720969751549464</v>
+        <v>0.01027818893652233</v>
       </c>
       <c r="J22" t="n">
-        <v>0.01251522112115162</v>
+        <v>0.007001422568540781</v>
       </c>
       <c r="K22" t="n">
-        <v>0.04129132843184687</v>
+        <v>0.03473767821508985</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.01812544560821288</v>
+        <v>-0.004574972477059985</v>
       </c>
       <c r="M22" t="n">
-        <v>0.004996501907510694</v>
+        <v>0.02696646619597313</v>
       </c>
       <c r="N22" t="inlineStr"/>
     </row>
@@ -1459,43 +1459,43 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.008648234172201</v>
+        <v>0.9990847970837572</v>
       </c>
       <c r="C23" t="n">
-        <v>1.018221565488804</v>
+        <v>1.03251106394107</v>
       </c>
       <c r="D23" t="n">
-        <v>1.001971892845191</v>
+        <v>1.00940998734646</v>
       </c>
       <c r="E23" t="n">
-        <v>1.014901433423474</v>
+        <v>1.017893652197353</v>
       </c>
       <c r="F23" t="n">
-        <v>1.032805471154091</v>
+        <v>1.043927138812035</v>
       </c>
       <c r="G23" t="n">
-        <v>1.050302278516815</v>
+        <v>1.067131839466267</v>
       </c>
       <c r="H23" t="n">
-        <v>0.9906451594755995</v>
+        <v>1.015127629913726</v>
       </c>
       <c r="I23" t="n">
-        <v>0.9962859444778585</v>
+        <v>1.010331190953037</v>
       </c>
       <c r="J23" t="n">
-        <v>1.01259386423722</v>
+        <v>1.007025989829323</v>
       </c>
       <c r="K23" t="n">
-        <v>1.042155670902067</v>
+        <v>1.035348078817911</v>
       </c>
       <c r="L23" t="n">
-        <v>0.9820378322978484</v>
+        <v>0.9954354767684461</v>
       </c>
       <c r="M23" t="n">
-        <v>1.005009005238799</v>
+        <v>1.027333351790567</v>
       </c>
       <c r="N23" t="n">
-        <v>1.280100273282632</v>
+        <v>1.136189565080878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>